<commit_message>
faster speed for INT8 with dp4a in v1.8
</commit_message>
<xml_diff>
--- a/nbench/list2025.xlsx
+++ b/nbench/list2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archive\github\benchmark\nbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E098E126-1FA6-4BF3-BD7C-8317BC1A3229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00E8BB2-AEBF-4029-B746-2D21ECC4CBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="615" windowWidth="23790" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="238">
   <si>
     <t>CPU</t>
   </si>
@@ -747,6 +747,12 @@
   </si>
   <si>
     <t>11.801s</t>
+  </si>
+  <si>
+    <t>Eigenbau 6 AI CUDA</t>
+  </si>
+  <si>
+    <t>i3-6100</t>
   </si>
 </sst>
 </file>
@@ -865,7 +871,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -903,6 +909,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -915,7 +922,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1197,11 +1204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67877F8F-8163-43CC-9F81-802504486149}">
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K58" sqref="K58"/>
+      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1283,7 @@
       <c r="D2" s="10">
         <v>0.54100000000000004</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="19">
         <v>0.95899999999999996</v>
       </c>
       <c r="F2" s="10">
@@ -1332,7 +1339,7 @@
       <c r="D3" s="10">
         <v>1.238</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="19">
         <v>1.33</v>
       </c>
       <c r="F3" s="10">
@@ -1355,7 +1362,7 @@
         <v>225</v>
       </c>
       <c r="M3" s="18">
-        <f t="shared" ref="M3:Q55" si="0">D3*1000</f>
+        <f t="shared" ref="M3:Q56" si="0">D3*1000</f>
         <v>1238</v>
       </c>
       <c r="N3" s="18">
@@ -1389,7 +1396,7 @@
       <c r="D4" s="10">
         <v>1.04</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="19">
         <v>1.6850000000000001</v>
       </c>
       <c r="F4" s="10">
@@ -1446,7 +1453,7 @@
       <c r="D5" s="10">
         <v>1.379</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="19">
         <v>1.712</v>
       </c>
       <c r="F5" s="10">
@@ -1503,7 +1510,7 @@
       <c r="D6" s="10">
         <v>1.024</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="19">
         <v>1.821</v>
       </c>
       <c r="F6" s="10">
@@ -1560,7 +1567,7 @@
       <c r="D7" s="10">
         <v>2.456</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="19">
         <v>3.1059999999999999</v>
       </c>
       <c r="F7" s="10">
@@ -1615,7 +1622,7 @@
       <c r="D8" s="10">
         <v>2.7480000000000002</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="19">
         <v>3.282</v>
       </c>
       <c r="F8" s="10">
@@ -1672,7 +1679,7 @@
       <c r="D9" s="10">
         <v>4.7089999999999996</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="19">
         <v>5.1639999999999997</v>
       </c>
       <c r="F9" s="10">
@@ -1729,7 +1736,7 @@
       <c r="D10" s="10">
         <v>3.665</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="19">
         <v>5.46</v>
       </c>
       <c r="F10" s="10">
@@ -1786,7 +1793,7 @@
       <c r="D11" s="10">
         <v>4.665</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="19">
         <v>6.4809999999999999</v>
       </c>
       <c r="F11" s="10">
@@ -1843,7 +1850,7 @@
       <c r="D12" s="10">
         <v>5.7990000000000004</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="19">
         <v>6.7169999999999996</v>
       </c>
       <c r="F12" s="10">
@@ -1900,7 +1907,7 @@
       <c r="D13" s="10">
         <v>6.21</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="19">
         <v>7.0469999999999997</v>
       </c>
       <c r="F13" s="10">
@@ -1957,7 +1964,7 @@
       <c r="D14" s="10">
         <v>7.2430000000000003</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="19">
         <v>7.109</v>
       </c>
       <c r="F14" s="10">
@@ -2014,7 +2021,7 @@
       <c r="D15" s="10">
         <v>9.3940000000000001</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="19">
         <v>7.5289999999999999</v>
       </c>
       <c r="F15" s="10">
@@ -2071,7 +2078,7 @@
       <c r="D16" s="10">
         <v>7.7519999999999998</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="19">
         <v>7.5789999999999997</v>
       </c>
       <c r="F16" s="10">
@@ -2128,7 +2135,7 @@
       <c r="D17" s="10">
         <v>9.3859999999999992</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="19">
         <v>8.39</v>
       </c>
       <c r="F17" s="10">
@@ -2185,7 +2192,7 @@
       <c r="D18" s="10">
         <v>6.78</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="19">
         <v>9.5239999999999991</v>
       </c>
       <c r="F18" s="10">
@@ -2242,7 +2249,7 @@
       <c r="D19" s="10">
         <v>4.5910000000000002</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="19">
         <v>9.8949999999999996</v>
       </c>
       <c r="F19" s="10">
@@ -2299,7 +2306,7 @@
       <c r="D20" s="10">
         <v>8.68</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="19">
         <v>10.948</v>
       </c>
       <c r="F20" s="10">
@@ -2356,7 +2363,7 @@
       <c r="D21" s="10">
         <v>11.269</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="19">
         <v>11.927</v>
       </c>
       <c r="F21" s="10">
@@ -2413,7 +2420,7 @@
       <c r="D22" s="10">
         <v>12.138</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="19">
         <v>12.568</v>
       </c>
       <c r="F22" s="10">
@@ -2470,7 +2477,7 @@
       <c r="D23" s="10">
         <v>18.433</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="19">
         <v>15.15</v>
       </c>
       <c r="F23" s="10">
@@ -2527,7 +2534,7 @@
       <c r="D24" s="10">
         <v>14.398999999999999</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="19">
         <v>15.946999999999999</v>
       </c>
       <c r="F24" s="10">
@@ -2582,7 +2589,7 @@
       <c r="D25" s="10">
         <v>13.595000000000001</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="19">
         <v>16.120999999999999</v>
       </c>
       <c r="F25" s="10">
@@ -2639,7 +2646,7 @@
       <c r="D26" s="10">
         <v>19.981000000000002</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="19">
         <v>16.207000000000001</v>
       </c>
       <c r="F26" s="10">
@@ -2696,7 +2703,7 @@
       <c r="D27" s="10">
         <v>19.050999999999998</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="19">
         <v>17.286000000000001</v>
       </c>
       <c r="F27" s="10">
@@ -2753,7 +2760,7 @@
       <c r="D28" s="10">
         <v>28.488</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="19">
         <v>17.780999999999999</v>
       </c>
       <c r="F28" s="10">
@@ -2810,7 +2817,7 @@
       <c r="D29" s="10">
         <v>23.695</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="19">
         <v>17.817</v>
       </c>
       <c r="F29" s="10">
@@ -2867,7 +2874,7 @@
       <c r="D30" s="10">
         <v>18.776</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="19">
         <v>17.878</v>
       </c>
       <c r="F30" s="10">
@@ -2924,7 +2931,7 @@
       <c r="D31" s="10">
         <v>15.319000000000001</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="19">
         <v>18.061</v>
       </c>
       <c r="F31" s="10">
@@ -2981,7 +2988,7 @@
       <c r="D32" s="10">
         <v>18.265000000000001</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="19">
         <v>18.957999999999998</v>
       </c>
       <c r="F32" s="10">
@@ -3038,7 +3045,7 @@
       <c r="D33" s="10">
         <v>14.395</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="19">
         <v>19.298999999999999</v>
       </c>
       <c r="F33" s="10">
@@ -3095,7 +3102,7 @@
       <c r="D34" s="10">
         <v>28.631</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="19">
         <v>19.780999999999999</v>
       </c>
       <c r="F34" s="10">
@@ -3152,7 +3159,7 @@
       <c r="D35" s="10">
         <v>19.359000000000002</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="19">
         <v>19.808</v>
       </c>
       <c r="F35" s="10">
@@ -3209,7 +3216,7 @@
       <c r="D36" s="10">
         <v>33.670999999999999</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="19">
         <v>23.584</v>
       </c>
       <c r="F36" s="10">
@@ -3266,7 +3273,7 @@
       <c r="D37" s="10">
         <v>28.776</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="19">
         <v>23.881</v>
       </c>
       <c r="F37" s="10">
@@ -3323,7 +3330,7 @@
       <c r="D38" s="10">
         <v>37.845999999999997</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="19">
         <v>23.882000000000001</v>
       </c>
       <c r="F38" s="10">
@@ -3380,7 +3387,7 @@
       <c r="D39" s="10">
         <v>24.206</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="19">
         <v>24.602</v>
       </c>
       <c r="F39" s="10">
@@ -3431,7 +3438,7 @@
       <c r="D40" s="10">
         <v>21.475999999999999</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="19">
         <v>25.608000000000001</v>
       </c>
       <c r="F40" s="10">
@@ -3488,7 +3495,7 @@
       <c r="D41" s="10">
         <v>27.460999999999999</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="19">
         <v>26.341999999999999</v>
       </c>
       <c r="F41" s="10">
@@ -3545,7 +3552,7 @@
       <c r="D42" s="10">
         <v>28.021999999999998</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="19">
         <v>32.585999999999999</v>
       </c>
       <c r="F42" s="10">
@@ -3602,7 +3609,7 @@
       <c r="D43" s="10">
         <v>39.049999999999997</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="19">
         <v>33.215000000000003</v>
       </c>
       <c r="F43" s="10">
@@ -3659,7 +3666,7 @@
       <c r="D44" s="10">
         <v>40.698999999999998</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="19">
         <v>37.018000000000001</v>
       </c>
       <c r="F44" s="10">
@@ -3716,7 +3723,7 @@
       <c r="D45" s="10">
         <v>45.381999999999998</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E45" s="19">
         <v>40.313000000000002</v>
       </c>
       <c r="F45" s="10">
@@ -3773,7 +3780,7 @@
       <c r="D46" s="10">
         <v>57.2</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="19">
         <v>43.731999999999999</v>
       </c>
       <c r="F46" s="10">
@@ -3830,7 +3837,7 @@
       <c r="D47" s="10">
         <v>55.045999999999999</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="19">
         <v>44.618000000000002</v>
       </c>
       <c r="F47" s="10">
@@ -3887,7 +3894,7 @@
       <c r="D48" s="10">
         <v>63.682000000000002</v>
       </c>
-      <c r="E48" s="23">
+      <c r="E48" s="19">
         <v>45.731999999999999</v>
       </c>
       <c r="F48" s="10">
@@ -3944,7 +3951,7 @@
       <c r="D49" s="10">
         <v>50.423000000000002</v>
       </c>
-      <c r="E49" s="23">
+      <c r="E49" s="19">
         <v>46.116999999999997</v>
       </c>
       <c r="F49" s="10">
@@ -4001,7 +4008,7 @@
       <c r="D50" s="10">
         <v>61.249000000000002</v>
       </c>
-      <c r="E50" s="23">
+      <c r="E50" s="19">
         <v>46.226999999999997</v>
       </c>
       <c r="F50" s="10">
@@ -4024,7 +4031,7 @@
         <v>223</v>
       </c>
       <c r="M50" s="18">
-        <f t="shared" ref="M50:Q50" si="2">D50*1000</f>
+        <f t="shared" ref="M50:Q51" si="2">D50*1000</f>
         <v>61249</v>
       </c>
       <c r="N50" s="18">
@@ -4046,306 +4053,357 @@
       <c r="R50" s="18"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>234</v>
-      </c>
-      <c r="B51" t="s">
-        <v>233</v>
-      </c>
-      <c r="C51">
-        <v>2295</v>
+      <c r="A51" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="C51" s="24">
+        <v>3700</v>
       </c>
       <c r="D51" s="10">
-        <v>59.665999999999997</v>
-      </c>
-      <c r="E51" s="23">
-        <v>49.441000000000003</v>
+        <v>68.150000000000006</v>
+      </c>
+      <c r="E51" s="19">
+        <v>48.103000000000002</v>
       </c>
       <c r="F51" s="10">
-        <v>116.922</v>
+        <v>118.447</v>
       </c>
       <c r="G51" s="11">
-        <v>214.8</v>
+        <v>223.80500000000001</v>
       </c>
       <c r="H51" s="11">
-        <v>210.8</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>235</v>
-      </c>
+        <v>216.554</v>
+      </c>
+      <c r="I51" s="8"/>
       <c r="J51" s="14">
-        <v>45298</v>
+        <v>45773</v>
       </c>
       <c r="K51" s="14"/>
       <c r="L51" s="5" t="s">
         <v>223</v>
       </c>
       <c r="M51" s="18">
-        <f t="shared" ref="M51" si="3">D51*1000</f>
-        <v>59666</v>
+        <f t="shared" si="2"/>
+        <v>68150</v>
       </c>
       <c r="N51" s="18">
-        <f t="shared" ref="N51" si="4">E51*1000</f>
-        <v>49441</v>
+        <f t="shared" si="2"/>
+        <v>48103</v>
       </c>
       <c r="O51" s="18">
-        <f t="shared" ref="O51" si="5">F51*1000</f>
-        <v>116922</v>
+        <f t="shared" si="2"/>
+        <v>118447</v>
       </c>
       <c r="P51" s="18">
-        <f t="shared" ref="P51" si="6">G51*1000</f>
-        <v>214800</v>
+        <f t="shared" si="2"/>
+        <v>223805</v>
       </c>
       <c r="Q51" s="18">
-        <f t="shared" ref="Q51" si="7">H51*1000</f>
-        <v>210800</v>
+        <f t="shared" si="2"/>
+        <v>216554</v>
       </c>
       <c r="R51" s="18"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="B52" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="C52">
-        <v>3700</v>
+        <v>2295</v>
       </c>
       <c r="D52" s="10">
-        <v>62.206000000000003</v>
-      </c>
-      <c r="E52" s="23">
-        <v>49.951000000000001</v>
+        <v>59.665999999999997</v>
+      </c>
+      <c r="E52" s="19">
+        <v>49.441000000000003</v>
       </c>
       <c r="F52" s="10">
-        <v>112.593</v>
+        <v>116.922</v>
       </c>
       <c r="G52" s="11">
-        <v>219.9</v>
+        <v>214.8</v>
       </c>
       <c r="H52" s="11">
-        <v>203</v>
+        <v>210.8</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="J52" s="13">
-        <v>45561</v>
-      </c>
-      <c r="K52" s="13"/>
+        <v>235</v>
+      </c>
+      <c r="J52" s="14">
+        <v>45298</v>
+      </c>
+      <c r="K52" s="14"/>
       <c r="L52" s="5" t="s">
         <v>223</v>
       </c>
       <c r="M52" s="18">
-        <f t="shared" si="0"/>
-        <v>62206</v>
+        <f t="shared" ref="M52" si="3">D52*1000</f>
+        <v>59666</v>
       </c>
       <c r="N52" s="18">
-        <f t="shared" si="0"/>
-        <v>49951</v>
+        <f t="shared" ref="N52" si="4">E52*1000</f>
+        <v>49441</v>
       </c>
       <c r="O52" s="18">
-        <f t="shared" si="0"/>
-        <v>112593</v>
+        <f t="shared" ref="O52" si="5">F52*1000</f>
+        <v>116922</v>
       </c>
       <c r="P52" s="18">
-        <f t="shared" si="0"/>
-        <v>219900</v>
+        <f t="shared" ref="P52" si="6">G52*1000</f>
+        <v>214800</v>
       </c>
       <c r="Q52" s="18">
-        <f t="shared" si="0"/>
-        <v>203000</v>
+        <f t="shared" ref="Q52" si="7">H52*1000</f>
+        <v>210800</v>
       </c>
       <c r="R52" s="18"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="B53" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="C53">
-        <v>4160</v>
+        <v>3700</v>
       </c>
       <c r="D53" s="10">
-        <v>77.174000000000007</v>
-      </c>
-      <c r="E53" s="23">
-        <v>56.761000000000003</v>
+        <v>62.206000000000003</v>
+      </c>
+      <c r="E53" s="19">
+        <v>49.951000000000001</v>
       </c>
       <c r="F53" s="10">
-        <v>138.00299999999999</v>
+        <v>112.593</v>
       </c>
       <c r="G53" s="11">
-        <v>259.47000000000003</v>
+        <v>219.9</v>
       </c>
       <c r="H53" s="11">
-        <v>248.81200000000001</v>
+        <v>203</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="J53" s="14">
-        <v>45211</v>
-      </c>
-      <c r="K53" s="14"/>
+        <v>207</v>
+      </c>
+      <c r="J53" s="13">
+        <v>45561</v>
+      </c>
+      <c r="K53" s="13"/>
       <c r="L53" s="5" t="s">
         <v>223</v>
       </c>
       <c r="M53" s="18">
         <f t="shared" si="0"/>
-        <v>77174</v>
+        <v>62206</v>
       </c>
       <c r="N53" s="18">
         <f t="shared" si="0"/>
-        <v>56761</v>
+        <v>49951</v>
       </c>
       <c r="O53" s="18">
         <f t="shared" si="0"/>
-        <v>138003</v>
+        <v>112593</v>
       </c>
       <c r="P53" s="18">
         <f t="shared" si="0"/>
-        <v>259470.00000000003</v>
+        <v>219900</v>
       </c>
       <c r="Q53" s="18">
         <f t="shared" si="0"/>
-        <v>248812</v>
+        <v>203000</v>
       </c>
       <c r="R53" s="18"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="C54" s="16">
-        <v>3200</v>
+      <c r="A54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54">
+        <v>4160</v>
       </c>
       <c r="D54" s="10">
-        <v>66.938999999999993</v>
-      </c>
-      <c r="E54" s="23">
-        <v>79.733000000000004</v>
+        <v>77.174000000000007</v>
+      </c>
+      <c r="E54" s="19">
+        <v>56.761000000000003</v>
       </c>
       <c r="F54" s="10">
-        <v>216.304</v>
+        <v>138.00299999999999</v>
       </c>
       <c r="G54" s="11">
-        <v>296.39999999999998</v>
+        <v>259.47000000000003</v>
       </c>
       <c r="H54" s="11">
-        <v>389.9</v>
+        <v>248.81200000000001</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>10</v>
+        <v>195</v>
       </c>
       <c r="J54" s="14">
-        <v>45561</v>
+        <v>45211</v>
       </c>
       <c r="K54" s="14"/>
       <c r="L54" s="5" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="M54" s="18">
         <f t="shared" si="0"/>
-        <v>66939</v>
+        <v>77174</v>
       </c>
       <c r="N54" s="18">
         <f t="shared" si="0"/>
-        <v>79733</v>
+        <v>56761</v>
       </c>
       <c r="O54" s="18">
         <f t="shared" si="0"/>
-        <v>216304</v>
+        <v>138003</v>
       </c>
       <c r="P54" s="18">
         <f t="shared" si="0"/>
-        <v>296400</v>
+        <v>259470.00000000003</v>
       </c>
       <c r="Q54" s="18">
         <f t="shared" si="0"/>
-        <v>389900</v>
+        <v>248812</v>
       </c>
       <c r="R54" s="18"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>184</v>
-      </c>
-      <c r="B55" t="s">
-        <v>185</v>
-      </c>
-      <c r="C55">
-        <v>4700</v>
+      <c r="A55" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C55" s="16">
+        <v>3200</v>
       </c>
       <c r="D55" s="10">
-        <v>104.52500000000001</v>
-      </c>
-      <c r="E55" s="23">
-        <v>85.01</v>
+        <v>66.938999999999993</v>
+      </c>
+      <c r="E55" s="19">
+        <v>79.733000000000004</v>
       </c>
       <c r="F55" s="10">
-        <v>264.86900000000003</v>
+        <v>216.304</v>
       </c>
       <c r="G55" s="11">
-        <v>372.2</v>
+        <v>296.39999999999998</v>
       </c>
       <c r="H55" s="11">
-        <v>377.5</v>
+        <v>389.9</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>194</v>
+        <v>10</v>
       </c>
       <c r="J55" s="14">
         <v>45561</v>
       </c>
       <c r="K55" s="14"/>
       <c r="L55" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="M55" s="18">
+        <f t="shared" si="0"/>
+        <v>66939</v>
+      </c>
+      <c r="N55" s="18">
+        <f t="shared" si="0"/>
+        <v>79733</v>
+      </c>
+      <c r="O55" s="18">
+        <f t="shared" si="0"/>
+        <v>216304</v>
+      </c>
+      <c r="P55" s="18">
+        <f t="shared" si="0"/>
+        <v>296400</v>
+      </c>
+      <c r="Q55" s="18">
+        <f t="shared" si="0"/>
+        <v>389900</v>
+      </c>
+      <c r="R55" s="18"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56">
+        <v>4700</v>
+      </c>
+      <c r="D56" s="10">
+        <v>104.52500000000001</v>
+      </c>
+      <c r="E56" s="19">
+        <v>85.01</v>
+      </c>
+      <c r="F56" s="10">
+        <v>264.86900000000003</v>
+      </c>
+      <c r="G56" s="11">
+        <v>372.2</v>
+      </c>
+      <c r="H56" s="11">
+        <v>377.5</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="J56" s="14">
+        <v>45561</v>
+      </c>
+      <c r="K56" s="14"/>
+      <c r="L56" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="M55" s="18">
+      <c r="M56" s="18">
         <f t="shared" si="0"/>
         <v>104525</v>
       </c>
-      <c r="N55" s="18">
+      <c r="N56" s="18">
         <f t="shared" si="0"/>
         <v>85010</v>
       </c>
-      <c r="O55" s="18">
+      <c r="O56" s="18">
         <f t="shared" si="0"/>
         <v>264869</v>
       </c>
-      <c r="P55" s="18">
+      <c r="P56" s="18">
         <f t="shared" si="0"/>
         <v>372200</v>
       </c>
-      <c r="Q55" s="18">
+      <c r="Q56" s="18">
         <f t="shared" si="0"/>
         <v>377500</v>
       </c>
-      <c r="R55" s="18"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
+      <c r="R56" s="18"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
       <c r="F57" s="10"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F58" s="10"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
@@ -4356,6 +4414,10 @@
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11842,7 +11904,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -11854,10 +11916,10 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -11865,7 +11927,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -11875,8 +11937,8 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
@@ -12023,22 +12085,22 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="22">
         <v>2.7480000000000002</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="22">
         <v>3.282</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="22">
         <v>3.7109999999999999</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="23">
         <v>12.8</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="23">
         <v>6.69</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="22" t="s">
         <v>10</v>
       </c>
     </row>
@@ -12046,33 +12108,33 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="22">
         <v>3.665</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="22">
         <v>5.46</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="22">
         <v>4.6849999999999996</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="23">
         <v>18.399999999999999</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="23">
         <v>8.4499999999999993</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="22" t="s">
         <v>10</v>
       </c>
     </row>
@@ -12080,12 +12142,12 @@
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -12229,22 +12291,22 @@
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="22">
         <v>4.5910000000000002</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="22">
         <v>9.8949999999999996</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="22">
         <v>9.0860000000000003</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="23">
         <v>28.5</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="23">
         <v>16.399999999999999</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="22" t="s">
         <v>10</v>
       </c>
     </row>
@@ -12252,12 +12314,12 @@
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="22"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -12881,7 +12943,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -12893,10 +12955,10 @@
       <c r="D48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="21" t="s">
         <v>6</v>
       </c>
       <c r="G48" s="1" t="s">
@@ -12904,7 +12966,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="1" t="s">
         <v>2</v>
       </c>
@@ -12914,14 +12976,30 @@
       <c r="D49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
       <c r="G49" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="F48:F49"/>
@@ -12930,22 +13008,6 @@
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="http://pdadb.net/index.php?m=cpu&amp;id=a6422&amp;c=samsung_s5p6422" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>